<commit_message>
Update Waste model version
</commit_message>
<xml_diff>
--- a/Waste/A1_Outputs/A-O_AR_Projections_COMPLETED.xlsx
+++ b/Waste/A1_Outputs/A-O_AR_Projections_COMPLETED.xlsx
@@ -5432,13 +5432,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9B2885A-E016-4777-AE7D-8295A487BF46}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2578B2DA-8799-4C47-B43C-437D7148D569}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8160B13-4D65-4C68-BA0C-E44288210DF2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7230436-461C-4CB6-B323-61F8594F4383}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2E875ED-FFEA-46BC-B596-AB821BDB5D8D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B17F09E-32F9-4015-907C-EEB103645811}"/>
 </file>
</xml_diff>